<commit_message>
update data dictionary and add clustering file
</commit_message>
<xml_diff>
--- a/policeData/policeStopsDataDictionary.xlsx
+++ b/policeData/policeStopsDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dillon\projects\SDTechHub\policeData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20145A39-F5FD-4C13-894E-E807F0B178F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA745A6-0CDB-45A2-AC8D-3552E945A1E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23970" yWindow="4665" windowWidth="35115" windowHeight="15705" xr2:uid="{0357B36F-E8D3-434D-A299-43A4CDACF8AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35115" windowHeight="15705" xr2:uid="{0357B36F-E8D3-434D-A299-43A4CDACF8AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="108">
   <si>
     <t>field</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Yes or blank</t>
   </si>
   <si>
-    <t>basisforpropertyseizure</t>
-  </si>
-  <si>
     <t>basis for property seizure</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>brief narrative explaining the reason for the stop</t>
   </si>
   <si>
-    <t>resultkey</t>
-  </si>
-  <si>
     <t>outcome(s) of stop (code)</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>see resultText attribute for descriptions of codes</t>
   </si>
   <si>
-    <t>resulttext</t>
-  </si>
-  <si>
     <t>specific violation if stop outcome is warning, citation or custodial arrest (description)</t>
   </si>
   <si>
@@ -213,24 +204,15 @@
     <t>officer years of experience in law enforcement</t>
   </si>
   <si>
-    <t>stopdate</t>
-  </si>
-  <si>
     <t>datetime64[ns]</t>
   </si>
   <si>
     <t>date  stop occurred</t>
   </si>
   <si>
-    <t>stoptime</t>
-  </si>
-  <si>
     <t>time stop began</t>
   </si>
   <si>
-    <t>stopduration</t>
-  </si>
-  <si>
     <t>duration of time for stop in minutes</t>
   </si>
   <si>
@@ -264,21 +246,12 @@
     <t>location of stop - intersecting street name</t>
   </si>
   <si>
-    <t>block</t>
-  </si>
-  <si>
     <t>location of stop - hundred block</t>
   </si>
   <si>
-    <t>land_mark</t>
-  </si>
-  <si>
     <t>location of stop - landmark</t>
   </si>
   <si>
-    <t>street</t>
-  </si>
-  <si>
     <t>location of stop - street name</t>
   </si>
   <si>
@@ -288,9 +261,6 @@
     <t>location of stop - highway exit</t>
   </si>
   <si>
-    <t>isschool</t>
-  </si>
-  <si>
     <t>did stop occur at a school?</t>
   </si>
   <si>
@@ -300,9 +270,6 @@
     <t>name of school where stop occurred</t>
   </si>
   <si>
-    <t>cityname</t>
-  </si>
-  <si>
     <t>name of city where stop occurred</t>
   </si>
   <si>
@@ -321,9 +288,6 @@
     <t>location of stop - SDPD beat/neighborhood name</t>
   </si>
   <si>
-    <t>isstudent</t>
-  </si>
-  <si>
     <t>was person stopped a student?</t>
   </si>
   <si>
@@ -351,21 +315,6 @@
     <t>officer's perception of whether the person stopped is gender nonconforming</t>
   </si>
   <si>
-    <t>gend</t>
-  </si>
-  <si>
-    <t>officer's perception of the gender of the person stopped (code)</t>
-  </si>
-  <si>
-    <t>see perceivedGender attribute for descriptions related to codes</t>
-  </si>
-  <si>
-    <t>gend_nc</t>
-  </si>
-  <si>
-    <t>No data = No, 5 = Yes</t>
-  </si>
-  <si>
     <t>perceived_lgbt</t>
   </si>
   <si>
@@ -373,6 +322,42 @@
   </si>
   <si>
     <t>Yes, No</t>
+  </si>
+  <si>
+    <t>basis_for_property_seizure</t>
+  </si>
+  <si>
+    <t>date_stop</t>
+  </si>
+  <si>
+    <t>time_stop</t>
+  </si>
+  <si>
+    <t>stop_duration</t>
+  </si>
+  <si>
+    <t>is_student</t>
+  </si>
+  <si>
+    <t>is_school</t>
+  </si>
+  <si>
+    <t>landmark</t>
+  </si>
+  <si>
+    <t>address_block</t>
+  </si>
+  <si>
+    <t>address_city</t>
+  </si>
+  <si>
+    <t>result_text</t>
+  </si>
+  <si>
+    <t>result_key</t>
+  </si>
+  <si>
+    <t>address_street</t>
   </si>
 </sst>
 </file>
@@ -733,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B64253-8906-47E8-B8BD-0D763FAEF260}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,13 +798,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -827,13 +812,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -841,24 +826,24 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -866,13 +851,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -880,13 +865,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -894,13 +879,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -908,13 +893,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -922,38 +907,38 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -961,38 +946,38 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1000,138 +985,138 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -1139,168 +1124,168 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D42" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -1308,58 +1293,30 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D46" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>110</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>111</v>
-      </c>
-      <c r="D48" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>